<commit_message>
completed 2 till demo
</commit_message>
<xml_diff>
--- a/output_final.xlsx
+++ b/output_final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Listen_start</t>
   </si>
@@ -34,28 +34,32 @@
     <t>start_diff</t>
   </si>
   <si>
-    <t>1539.9161937</t>
-  </si>
-  <si>
-    <t>1562.0225384</t>
-  </si>
-  <si>
-    <t>1541.0589795</t>
-  </si>
-  <si>
-    <t>1562.2117658</t>
-  </si>
-  <si>
-    <t>1551.4564884</t>
-  </si>
-  <si>
-    <t>1573.505146</t>
-  </si>
-  <si>
-    <t>1558.2989893</t>
-  </si>
-  <si>
-    <t>1575.8329155</t>
+    <t>4799.8950226</t>
+  </si>
+  <si>
+    <t>4822.0594192</t>
+  </si>
+  <si>
+    <t>4800.025131</t>
+  </si>
+  <si>
+    <t>4822.0235126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365_x000D_
+</t>
+  </si>
+  <si>
+    <t>4811.4082363</t>
+  </si>
+  <si>
+    <t>4833.5408547</t>
+  </si>
+  <si>
+    <t>4813.4254384</t>
+  </si>
+  <si>
+    <t>4836.8184474</t>
   </si>
 </sst>
 </file>
@@ -446,17 +450,17 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>1250</v>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2">
-        <v>1.142785800000183</v>
+        <v>0.1301084000006085</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -466,17 +470,17 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>1250</v>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3">
-        <v>0.1892273999999361</v>
+        <v>-0.03590660000008938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete demo - 28/4
</commit_message>
<xml_diff>
--- a/output_final.xlsx
+++ b/output_final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Listen_start</t>
   </si>
@@ -34,32 +34,28 @@
     <t>start_diff</t>
   </si>
   <si>
-    <t>4799.8950226</t>
-  </si>
-  <si>
-    <t>4822.0594192</t>
-  </si>
-  <si>
-    <t>4800.025131</t>
-  </si>
-  <si>
-    <t>4822.0235126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">365_x000D_
-</t>
-  </si>
-  <si>
-    <t>4811.4082363</t>
-  </si>
-  <si>
-    <t>4833.5408547</t>
-  </si>
-  <si>
-    <t>4813.4254384</t>
-  </si>
-  <si>
-    <t>4836.8184474</t>
+    <t>8917.1622553</t>
+  </si>
+  <si>
+    <t>8981.6220102</t>
+  </si>
+  <si>
+    <t>8918.401366</t>
+  </si>
+  <si>
+    <t>8981.656001</t>
+  </si>
+  <si>
+    <t>8930.6574626</t>
+  </si>
+  <si>
+    <t>8995.0509062</t>
+  </si>
+  <si>
+    <t>8967.0377007</t>
+  </si>
+  <si>
+    <t>9031.1469414</t>
   </si>
 </sst>
 </file>
@@ -450,17 +446,17 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>144</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
-        <v>0.1301084000006085</v>
+        <v>1.23911070000031</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -470,17 +466,17 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
+      <c r="C3">
+        <v>307.2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3">
-        <v>-0.03590660000008938</v>
+        <v>0.03399079999871901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>